<commit_message>
tambahkan format status karyawan
</commit_message>
<xml_diff>
--- a/resources/views/laporan-absensi-karyawan/format_laporan_rekap_absensi_karyawan.xlsx
+++ b/resources/views/laporan-absensi-karyawan/format_laporan_rekap_absensi_karyawan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/muslimlife/Sites/localhost/app_simrs_absensi_finger/resources/views/laporan-absensi-karyawan/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C6FE9A3-49F1-7749-81F4-C86214496B9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{377A1A3E-DCC8-504B-A901-D6B23C1E4F9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="0" windowWidth="32000" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -106,7 +106,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -130,12 +130,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFCCCCCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFEAEAEA"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -152,6 +146,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA7A7A7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC8C7C7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -268,7 +274,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -282,6 +288,72 @@
     <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -294,80 +366,11 @@
     <xf numFmtId="49" fontId="2" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -377,9 +380,11 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
   <colors>
     <mruColors>
+      <color rgb="FFEAEAEA"/>
+      <color rgb="FFC8C7C7"/>
+      <color rgb="FFA7A7A7"/>
       <color rgb="FFF7D44D"/>
       <color rgb="FFF39791"/>
-      <color rgb="FFEAEAEA"/>
       <color rgb="FFCCCCCC"/>
       <color rgb="FFEEECE1"/>
     </mruColors>
@@ -684,21 +689,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AL11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4:AH5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11:AH11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.83203125" style="16" customWidth="1"/>
-    <col min="2" max="2" width="11.5" style="16" customWidth="1"/>
-    <col min="3" max="3" width="3.1640625" style="16" customWidth="1"/>
-    <col min="4" max="4" width="18.5" style="17" customWidth="1"/>
-    <col min="5" max="31" width="9.83203125" style="11" customWidth="1"/>
-    <col min="32" max="32" width="9.83203125" style="12" customWidth="1"/>
-    <col min="33" max="33" width="15.83203125" style="12" customWidth="1"/>
-    <col min="34" max="34" width="15" style="12" customWidth="1"/>
-    <col min="35" max="38" width="20.83203125" style="12"/>
+    <col min="1" max="1" width="6.83203125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="11.5" style="9" customWidth="1"/>
+    <col min="3" max="3" width="3.1640625" style="9" customWidth="1"/>
+    <col min="4" max="4" width="18.5" style="10" customWidth="1"/>
+    <col min="5" max="31" width="9.83203125" style="7" customWidth="1"/>
+    <col min="32" max="32" width="9.83203125" style="8" customWidth="1"/>
+    <col min="33" max="33" width="15.83203125" style="8" customWidth="1"/>
+    <col min="34" max="34" width="15" style="8" customWidth="1"/>
+    <col min="35" max="38" width="20.83203125" style="8"/>
     <col min="39" max="16384" width="20.83203125" style="2"/>
   </cols>
   <sheetData>
@@ -743,40 +748,40 @@
       <c r="AL1" s="2"/>
     </row>
     <row r="2" spans="1:38" ht="24" x14ac:dyDescent="0.2">
-      <c r="A2" s="30"/>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
-      <c r="O2" s="30"/>
-      <c r="P2" s="30"/>
-      <c r="Q2" s="30"/>
-      <c r="R2" s="30"/>
-      <c r="S2" s="30"/>
-      <c r="T2" s="30"/>
-      <c r="U2" s="30"/>
-      <c r="V2" s="30"/>
-      <c r="W2" s="30"/>
-      <c r="X2" s="30"/>
-      <c r="Y2" s="30"/>
-      <c r="Z2" s="30"/>
-      <c r="AA2" s="30"/>
-      <c r="AB2" s="30"/>
-      <c r="AC2" s="30"/>
-      <c r="AD2" s="30"/>
-      <c r="AE2" s="30"/>
-      <c r="AF2" s="30"/>
-      <c r="AG2" s="30"/>
-      <c r="AH2" s="30"/>
+      <c r="A2" s="27"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="27"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="27"/>
+      <c r="N2" s="27"/>
+      <c r="O2" s="27"/>
+      <c r="P2" s="27"/>
+      <c r="Q2" s="27"/>
+      <c r="R2" s="27"/>
+      <c r="S2" s="27"/>
+      <c r="T2" s="27"/>
+      <c r="U2" s="27"/>
+      <c r="V2" s="27"/>
+      <c r="W2" s="27"/>
+      <c r="X2" s="27"/>
+      <c r="Y2" s="27"/>
+      <c r="Z2" s="27"/>
+      <c r="AA2" s="27"/>
+      <c r="AB2" s="27"/>
+      <c r="AC2" s="27"/>
+      <c r="AD2" s="27"/>
+      <c r="AE2" s="27"/>
+      <c r="AF2" s="27"/>
+      <c r="AG2" s="27"/>
+      <c r="AH2" s="27"/>
       <c r="AI2" s="2"/>
       <c r="AJ2" s="2"/>
       <c r="AK2" s="2"/>
@@ -823,92 +828,92 @@
       <c r="AL3" s="2"/>
     </row>
     <row r="4" spans="1:38" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="13"/>
+      <c r="B4" s="28"/>
       <c r="C4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="32" t="s">
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="32"/>
-      <c r="J4" s="33"/>
-      <c r="K4" s="33"/>
-      <c r="L4" s="33"/>
-      <c r="M4" s="33"/>
-      <c r="N4" s="33"/>
-      <c r="O4" s="33"/>
-      <c r="P4" s="33"/>
-      <c r="Q4" s="33"/>
-      <c r="R4" s="33"/>
-      <c r="S4" s="33"/>
-      <c r="T4" s="33"/>
-      <c r="U4" s="33"/>
-      <c r="V4" s="33"/>
-      <c r="W4" s="33"/>
-      <c r="X4" s="33"/>
-      <c r="Y4" s="33"/>
-      <c r="Z4" s="33"/>
-      <c r="AA4" s="33"/>
-      <c r="AB4" s="33"/>
-      <c r="AC4" s="33"/>
-      <c r="AD4" s="33"/>
-      <c r="AE4" s="33"/>
-      <c r="AF4" s="33"/>
-      <c r="AG4" s="33"/>
-      <c r="AH4" s="33"/>
+      <c r="I4" s="23"/>
+      <c r="J4" s="25"/>
+      <c r="K4" s="25"/>
+      <c r="L4" s="25"/>
+      <c r="M4" s="25"/>
+      <c r="N4" s="25"/>
+      <c r="O4" s="25"/>
+      <c r="P4" s="25"/>
+      <c r="Q4" s="25"/>
+      <c r="R4" s="25"/>
+      <c r="S4" s="25"/>
+      <c r="T4" s="25"/>
+      <c r="U4" s="25"/>
+      <c r="V4" s="25"/>
+      <c r="W4" s="25"/>
+      <c r="X4" s="25"/>
+      <c r="Y4" s="25"/>
+      <c r="Z4" s="25"/>
+      <c r="AA4" s="25"/>
+      <c r="AB4" s="25"/>
+      <c r="AC4" s="25"/>
+      <c r="AD4" s="25"/>
+      <c r="AE4" s="25"/>
+      <c r="AF4" s="25"/>
+      <c r="AG4" s="25"/>
+      <c r="AH4" s="25"/>
       <c r="AI4" s="2"/>
       <c r="AJ4" s="2"/>
       <c r="AK4" s="2"/>
       <c r="AL4" s="2"/>
     </row>
     <row r="5" spans="1:38" ht="24" x14ac:dyDescent="0.2">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="13"/>
+      <c r="B5" s="28"/>
       <c r="C5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="27"/>
-      <c r="H5" s="31" t="s">
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="I5" s="31"/>
-      <c r="J5" s="34"/>
-      <c r="K5" s="34"/>
-      <c r="L5" s="34"/>
-      <c r="M5" s="34"/>
-      <c r="N5" s="34"/>
-      <c r="O5" s="34"/>
-      <c r="P5" s="34"/>
-      <c r="Q5" s="34"/>
-      <c r="R5" s="34"/>
-      <c r="S5" s="34"/>
-      <c r="T5" s="34"/>
-      <c r="U5" s="34"/>
-      <c r="V5" s="34"/>
-      <c r="W5" s="34"/>
-      <c r="X5" s="34"/>
-      <c r="Y5" s="34"/>
-      <c r="Z5" s="34"/>
-      <c r="AA5" s="34"/>
-      <c r="AB5" s="34"/>
-      <c r="AC5" s="34"/>
-      <c r="AD5" s="34"/>
-      <c r="AE5" s="34"/>
-      <c r="AF5" s="34"/>
-      <c r="AG5" s="34"/>
-      <c r="AH5" s="34"/>
+      <c r="I5" s="24"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="26"/>
+      <c r="M5" s="26"/>
+      <c r="N5" s="26"/>
+      <c r="O5" s="26"/>
+      <c r="P5" s="26"/>
+      <c r="Q5" s="26"/>
+      <c r="R5" s="26"/>
+      <c r="S5" s="26"/>
+      <c r="T5" s="26"/>
+      <c r="U5" s="26"/>
+      <c r="V5" s="26"/>
+      <c r="W5" s="26"/>
+      <c r="X5" s="26"/>
+      <c r="Y5" s="26"/>
+      <c r="Z5" s="26"/>
+      <c r="AA5" s="26"/>
+      <c r="AB5" s="26"/>
+      <c r="AC5" s="26"/>
+      <c r="AD5" s="26"/>
+      <c r="AE5" s="26"/>
+      <c r="AF5" s="26"/>
+      <c r="AG5" s="26"/>
+      <c r="AH5" s="26"/>
       <c r="AI5" s="2"/>
       <c r="AJ5" s="2"/>
       <c r="AK5" s="2"/>
@@ -955,46 +960,46 @@
       <c r="AL6" s="2"/>
     </row>
     <row r="7" spans="1:38" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="22"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="18"/>
-      <c r="L7" s="18"/>
-      <c r="M7" s="18"/>
-      <c r="N7" s="18"/>
-      <c r="O7" s="18"/>
-      <c r="P7" s="18"/>
-      <c r="Q7" s="18"/>
-      <c r="R7" s="18"/>
-      <c r="S7" s="18"/>
-      <c r="T7" s="18"/>
-      <c r="U7" s="18"/>
-      <c r="V7" s="18"/>
-      <c r="W7" s="18"/>
-      <c r="X7" s="18"/>
-      <c r="Y7" s="18"/>
-      <c r="Z7" s="18"/>
-      <c r="AA7" s="18"/>
-      <c r="AB7" s="18"/>
-      <c r="AC7" s="18"/>
-      <c r="AD7" s="18"/>
-      <c r="AE7" s="18"/>
-      <c r="AF7" s="18"/>
-      <c r="AG7" s="9" t="s">
+      <c r="C7" s="17"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="11"/>
+      <c r="O7" s="11"/>
+      <c r="P7" s="11"/>
+      <c r="Q7" s="11"/>
+      <c r="R7" s="11"/>
+      <c r="S7" s="11"/>
+      <c r="T7" s="11"/>
+      <c r="U7" s="11"/>
+      <c r="V7" s="11"/>
+      <c r="W7" s="11"/>
+      <c r="X7" s="11"/>
+      <c r="Y7" s="11"/>
+      <c r="Z7" s="11"/>
+      <c r="AA7" s="11"/>
+      <c r="AB7" s="11"/>
+      <c r="AC7" s="11"/>
+      <c r="AD7" s="11"/>
+      <c r="AE7" s="11"/>
+      <c r="AF7" s="11"/>
+      <c r="AG7" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="AH7" s="9" t="s">
+      <c r="AH7" s="31" t="s">
         <v>3</v>
       </c>
       <c r="AI7" s="2"/>
@@ -1003,138 +1008,168 @@
       <c r="AL7" s="2"/>
     </row>
     <row r="8" spans="1:38" s="4" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="8"/>
-      <c r="B8" s="24"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="19"/>
-      <c r="I8" s="19"/>
-      <c r="J8" s="19"/>
-      <c r="K8" s="19"/>
-      <c r="L8" s="19"/>
-      <c r="M8" s="19"/>
-      <c r="N8" s="19"/>
-      <c r="O8" s="19"/>
-      <c r="P8" s="19"/>
-      <c r="Q8" s="19"/>
-      <c r="R8" s="19"/>
-      <c r="S8" s="19"/>
-      <c r="T8" s="19"/>
-      <c r="U8" s="19"/>
-      <c r="V8" s="19"/>
-      <c r="W8" s="19"/>
-      <c r="X8" s="19"/>
-      <c r="Y8" s="19"/>
-      <c r="Z8" s="19"/>
-      <c r="AA8" s="19"/>
-      <c r="AB8" s="19"/>
-      <c r="AC8" s="19"/>
-      <c r="AD8" s="19"/>
-      <c r="AE8" s="19"/>
-      <c r="AF8" s="20"/>
-      <c r="AG8" s="10"/>
-      <c r="AH8" s="10"/>
+      <c r="A8" s="30"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="12"/>
+      <c r="N8" s="12"/>
+      <c r="O8" s="12"/>
+      <c r="P8" s="12"/>
+      <c r="Q8" s="12"/>
+      <c r="R8" s="12"/>
+      <c r="S8" s="12"/>
+      <c r="T8" s="12"/>
+      <c r="U8" s="12"/>
+      <c r="V8" s="12"/>
+      <c r="W8" s="12"/>
+      <c r="X8" s="12"/>
+      <c r="Y8" s="12"/>
+      <c r="Z8" s="12"/>
+      <c r="AA8" s="12"/>
+      <c r="AB8" s="12"/>
+      <c r="AC8" s="12"/>
+      <c r="AD8" s="12"/>
+      <c r="AE8" s="12"/>
+      <c r="AF8" s="13"/>
+      <c r="AG8" s="32"/>
+      <c r="AH8" s="32"/>
     </row>
     <row r="9" spans="1:38" ht="20" x14ac:dyDescent="0.2">
-      <c r="A9" s="14"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="14"/>
-      <c r="M9" s="14"/>
-      <c r="N9" s="14"/>
-      <c r="O9" s="14"/>
-      <c r="P9" s="14"/>
-      <c r="Q9" s="14"/>
-      <c r="R9" s="14"/>
-      <c r="S9" s="14"/>
-      <c r="T9" s="14"/>
-      <c r="U9" s="14"/>
-      <c r="V9" s="14"/>
-      <c r="W9" s="14"/>
-      <c r="X9" s="14"/>
-      <c r="Y9" s="14"/>
-      <c r="Z9" s="14"/>
-      <c r="AA9" s="14"/>
-      <c r="AB9" s="14"/>
-      <c r="AC9" s="14"/>
-      <c r="AD9" s="14"/>
-      <c r="AE9" s="14"/>
-      <c r="AF9" s="14"/>
-      <c r="AG9" s="14"/>
-      <c r="AH9" s="14"/>
+      <c r="A9" s="15"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="15"/>
+      <c r="N9" s="15"/>
+      <c r="O9" s="15"/>
+      <c r="P9" s="15"/>
+      <c r="Q9" s="15"/>
+      <c r="R9" s="15"/>
+      <c r="S9" s="15"/>
+      <c r="T9" s="15"/>
+      <c r="U9" s="15"/>
+      <c r="V9" s="15"/>
+      <c r="W9" s="15"/>
+      <c r="X9" s="15"/>
+      <c r="Y9" s="15"/>
+      <c r="Z9" s="15"/>
+      <c r="AA9" s="15"/>
+      <c r="AB9" s="15"/>
+      <c r="AC9" s="15"/>
+      <c r="AD9" s="15"/>
+      <c r="AE9" s="15"/>
+      <c r="AF9" s="15"/>
+      <c r="AG9" s="15"/>
+      <c r="AH9" s="15"/>
     </row>
     <row r="10" spans="1:38" ht="20" x14ac:dyDescent="0.2">
-      <c r="A10" s="5"/>
-      <c r="B10" s="28"/>
-      <c r="C10" s="28"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="28"/>
-      <c r="H10" s="28"/>
-      <c r="I10" s="28"/>
-      <c r="J10" s="28"/>
-      <c r="K10" s="28"/>
-      <c r="L10" s="28"/>
-      <c r="M10" s="28"/>
-      <c r="N10" s="28"/>
-      <c r="O10" s="28"/>
-      <c r="P10" s="28"/>
-      <c r="Q10" s="28"/>
-      <c r="R10" s="28"/>
-      <c r="S10" s="28"/>
-      <c r="T10" s="28"/>
-      <c r="U10" s="28"/>
-      <c r="V10" s="28"/>
-      <c r="W10" s="28"/>
-      <c r="X10" s="28"/>
-      <c r="Y10" s="28"/>
-      <c r="Z10" s="28"/>
-      <c r="AA10" s="28"/>
-      <c r="AB10" s="28"/>
-      <c r="AC10" s="28"/>
-      <c r="AD10" s="28"/>
-      <c r="AE10" s="28"/>
-      <c r="AF10" s="28"/>
-      <c r="AG10" s="28"/>
-      <c r="AH10" s="28"/>
+      <c r="A10" s="33"/>
+      <c r="B10" s="33"/>
+      <c r="C10" s="33"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="33"/>
+      <c r="I10" s="33"/>
+      <c r="J10" s="33"/>
+      <c r="K10" s="33"/>
+      <c r="L10" s="33"/>
+      <c r="M10" s="33"/>
+      <c r="N10" s="33"/>
+      <c r="O10" s="33"/>
+      <c r="P10" s="33"/>
+      <c r="Q10" s="33"/>
+      <c r="R10" s="33"/>
+      <c r="S10" s="33"/>
+      <c r="T10" s="33"/>
+      <c r="U10" s="33"/>
+      <c r="V10" s="33"/>
+      <c r="W10" s="33"/>
+      <c r="X10" s="33"/>
+      <c r="Y10" s="33"/>
+      <c r="Z10" s="33"/>
+      <c r="AA10" s="33"/>
+      <c r="AB10" s="33"/>
+      <c r="AC10" s="33"/>
+      <c r="AD10" s="33"/>
+      <c r="AE10" s="33"/>
+      <c r="AF10" s="33"/>
+      <c r="AG10" s="33"/>
+      <c r="AH10" s="33"/>
     </row>
-    <row r="11" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="B11" s="29"/>
-      <c r="C11" s="29"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="15"/>
+    <row r="11" spans="1:38" ht="20" x14ac:dyDescent="0.2">
+      <c r="A11" s="5"/>
+      <c r="B11" s="34"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="34"/>
+      <c r="I11" s="34"/>
+      <c r="J11" s="34"/>
+      <c r="K11" s="34"/>
+      <c r="L11" s="34"/>
+      <c r="M11" s="34"/>
+      <c r="N11" s="34"/>
+      <c r="O11" s="34"/>
+      <c r="P11" s="34"/>
+      <c r="Q11" s="34"/>
+      <c r="R11" s="34"/>
+      <c r="S11" s="34"/>
+      <c r="T11" s="34"/>
+      <c r="U11" s="34"/>
+      <c r="V11" s="34"/>
+      <c r="W11" s="34"/>
+      <c r="X11" s="34"/>
+      <c r="Y11" s="34"/>
+      <c r="Z11" s="34"/>
+      <c r="AA11" s="34"/>
+      <c r="AB11" s="34"/>
+      <c r="AC11" s="34"/>
+      <c r="AD11" s="34"/>
+      <c r="AE11" s="34"/>
+      <c r="AF11" s="34"/>
+      <c r="AG11" s="34"/>
+      <c r="AH11" s="34"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="16">
+    <mergeCell ref="A2:AH2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="AG7:AG8"/>
+    <mergeCell ref="AH7:AH8"/>
+    <mergeCell ref="A9:AH9"/>
+    <mergeCell ref="B7:D8"/>
+    <mergeCell ref="B11:AH11"/>
+    <mergeCell ref="A10:AH10"/>
     <mergeCell ref="D4:F4"/>
     <mergeCell ref="D5:F5"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="H5:I5"/>
     <mergeCell ref="J4:AH4"/>
     <mergeCell ref="J5:AH5"/>
-    <mergeCell ref="A2:AH2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="B10:AH10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="AG7:AG8"/>
-    <mergeCell ref="AH7:AH8"/>
-    <mergeCell ref="A9:AH9"/>
-    <mergeCell ref="B7:D8"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>